<commit_message>
test ump changes + adjustments
</commit_message>
<xml_diff>
--- a/changes/45-ammo.xlsx
+++ b/changes/45-ammo.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lingl\Documents\deadline-balancing\changes\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{63DF6CDE-BFB2-45E9-BD69-136ED777E1C5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C38474EF-CEFD-4B89-8098-793830C49468}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1045,7 +1045,7 @@
   <dimension ref="A1:AA16"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="H16" sqref="H16"/>
+      <selection activeCell="R16" sqref="R16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1601,7 +1601,7 @@
         <v>0.1</v>
       </c>
       <c r="I11" s="3">
-        <v>0.17</v>
+        <v>0.16</v>
       </c>
       <c r="J11" s="3">
         <v>100</v>
@@ -1613,7 +1613,7 @@
       </c>
       <c r="N11" s="1">
         <f>C11-D11*20-E11*0.8-F11*0.6-H11*5+(W11-22)*1+P11/300+S11*2</f>
-        <v>20.593333333333327</v>
+        <v>20.246666666666663</v>
       </c>
       <c r="P11">
         <v>1000</v>
@@ -1629,19 +1629,19 @@
       </c>
       <c r="T11">
         <f>T3*(1+I11)</f>
-        <v>50.309999999999995</v>
+        <v>49.879999999999995</v>
       </c>
       <c r="U11">
         <f t="shared" ref="U11:U14" si="2">U3*(1+I11)</f>
-        <v>44.459999999999994</v>
+        <v>44.08</v>
       </c>
       <c r="V11">
         <f>V3*(I11+1)</f>
-        <v>26.909999999999997</v>
+        <v>26.68</v>
       </c>
       <c r="W11">
         <f t="shared" si="1"/>
-        <v>40.559999999999995</v>
+        <v>40.213333333333331</v>
       </c>
     </row>
     <row r="12" spans="1:27" x14ac:dyDescent="0.25">

</xml_diff>